<commit_message>
Taxonomy matching using topic names data
</commit_message>
<xml_diff>
--- a/Data/Workbooks/3_best_matches_topic.xlsx
+++ b/Data/Workbooks/3_best_matches_topic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lynko\Desktop\Thesis\Data\Workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ACAF090-46BF-4218-A7BE-50519EB2CB40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA7C435-C5C6-46FB-8ACB-7D41F6D358D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1083,8 +1083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P214"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F212" sqref="F212"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3959,7 +3959,7 @@
       <c r="E58">
         <v>507</v>
       </c>
-      <c r="F58" s="2" t="s">
+      <c r="F58" s="1" t="s">
         <v>58</v>
       </c>
       <c r="G58">

</xml_diff>